<commit_message>
new update in track
</commit_message>
<xml_diff>
--- a/reports/Automation_Report.xlsx
+++ b/reports/Automation_Report.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="2026-01-07" r:id="rId3" sheetId="1"/>
+    <sheet name="2026-01-12" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="40">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -90,6 +91,48 @@
   </si>
   <si>
     <t>TOTAL TIME EXECUTED : 98 sec</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_ADI_08</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_ADI_08 | Verify that uploaded track inventory appears in Admin and User App | "TD_UI_Zlaata_ADI_08"</t>
+  </si>
+  <si>
+    <t>gowthamraj</t>
+  </si>
+  <si>
+    <t>FEATURE FILES: allImport</t>
+  </si>
+  <si>
+    <t>TOTAL TIME EXECUTED : 36 sec</t>
+  </si>
+  <si>
+    <t>TOTAL TEST CASE EXECUTED : 0</t>
+  </si>
+  <si>
+    <t>TOTAL FAILED : 0</t>
+  </si>
+  <si>
+    <t>TOTAL TIME EXECUTED : 0 sec</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>TOTAL PASSED : 1</t>
+  </si>
+  <si>
+    <t>TOTAL TIME EXECUTED : 30 sec</t>
+  </si>
+  <si>
+    <t>TOTAL TIME EXECUTED : 27 sec</t>
+  </si>
+  <si>
+    <t>TOTAL TIME EXECUTED : 33 sec</t>
+  </si>
+  <si>
+    <t>TOTAL TIME EXECUTED : 29 sec</t>
   </si>
 </sst>
 </file>
@@ -97,13 +140,58 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -171,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -182,6 +270,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -267,6 +382,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>147996</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="18288000" cy="9001125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O9"/>
@@ -446,4 +604,373 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.60546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="107.03515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.90234375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.765625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.1796875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.03515625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.19921875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="2.15234375"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="2.15234375"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="2.15234375"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="2.15234375"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="2.15234375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="2.15234375"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="1.0390625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="32">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="32">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>36.571</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N8" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>30.453</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s" s="15">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N9" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>27.879</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s" s="21">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>33.736</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>29.811</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s" s="27">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>27.823</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s" s="30">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="I13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>